<commit_message>
commit mj collection for LinkedIn and Facebook
</commit_message>
<xml_diff>
--- a/Doc/lianshumianjing.xlsx
+++ b/Doc/lianshumianjing.xlsx
@@ -80,9 +80,6 @@
     <t>Product of subset of an array</t>
   </si>
   <si>
-    <t>sparse vector dot</t>
-  </si>
-  <si>
     <t>factorial trailing zeroes</t>
   </si>
   <si>
@@ -504,6 +501,9 @@
   </si>
   <si>
     <t>find median in sorted matrix. (heap)</t>
+  </si>
+  <si>
+    <t>sparse vector dot -&gt; sparse matrix multi</t>
   </si>
 </sst>
 </file>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -883,7 +883,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -951,7 +951,7 @@
       <c r="A13" s="4">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -975,7 +975,7 @@
       <c r="A16" s="4">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1015,8 +1015,8 @@
       <c r="A21" s="4">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
+      <c r="B21" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1024,7 +1024,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,7 +1032,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1040,7 +1040,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1048,7 +1048,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1056,10 +1056,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
         <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1067,10 +1067,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1078,7 +1078,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1094,7 +1094,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1102,7 +1102,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1110,10 +1110,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1121,7 +1121,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1129,7 +1129,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1137,7 +1137,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1145,7 +1145,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1153,7 +1153,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1161,10 +1161,10 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1172,7 +1172,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1180,7 +1180,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="192" customHeight="1" x14ac:dyDescent="0.3">
@@ -1188,10 +1188,10 @@
         <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1199,10 +1199,10 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1210,10 +1210,10 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
         <v>45</v>
-      </c>
-      <c r="C43" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1221,7 +1221,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1229,10 +1229,10 @@
         <v>45</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
         <v>48</v>
-      </c>
-      <c r="C45" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1240,7 +1240,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1248,7 +1248,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1264,10 +1264,10 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
         <v>53</v>
-      </c>
-      <c r="C49" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
@@ -1275,7 +1275,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1283,10 +1283,10 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
         <v>56</v>
-      </c>
-      <c r="C51" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1294,7 +1294,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1302,7 +1302,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1310,10 +1310,10 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" t="s">
         <v>60</v>
-      </c>
-      <c r="C54" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1321,10 +1321,10 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1332,10 +1332,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1343,10 +1343,10 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" t="s">
         <v>66</v>
-      </c>
-      <c r="C57" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1354,7 +1354,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="97.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1362,10 +1362,10 @@
         <v>59</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1373,7 +1373,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1381,7 +1381,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1389,10 +1389,10 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1400,10 +1400,10 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
         <v>73</v>
-      </c>
-      <c r="C63" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1411,10 +1411,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" t="s">
         <v>75</v>
-      </c>
-      <c r="C64" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1422,10 +1422,10 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" t="s">
         <v>77</v>
-      </c>
-      <c r="C65" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1433,7 +1433,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1441,7 +1441,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1449,10 +1449,10 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1460,10 +1460,10 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
         <v>83</v>
-      </c>
-      <c r="C69" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1471,7 +1471,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1479,7 +1479,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="121.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1487,10 +1487,10 @@
         <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1498,10 +1498,10 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" t="s">
         <v>89</v>
-      </c>
-      <c r="C73" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1509,7 +1509,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1517,7 +1517,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1525,7 +1525,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1533,10 +1533,10 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -1544,10 +1544,10 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="1" customFormat="1" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1555,7 +1555,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -1563,10 +1563,10 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
+        <v>96</v>
+      </c>
+      <c r="C80" t="s">
         <v>97</v>
-      </c>
-      <c r="C80" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -1574,7 +1574,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -1582,7 +1582,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="1" customFormat="1" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1590,7 +1590,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -1598,10 +1598,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C84" t="s">
         <v>102</v>
-      </c>
-      <c r="C84" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -1609,7 +1609,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
@@ -1617,7 +1617,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -1625,7 +1625,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -1633,10 +1633,10 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" t="s">
         <v>107</v>
-      </c>
-      <c r="C88" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -1644,7 +1644,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -1652,7 +1652,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="67.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1660,10 +1660,10 @@
         <v>91</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -1671,7 +1671,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1687,7 +1687,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -1695,7 +1695,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -1703,7 +1703,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -1711,10 +1711,10 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C97" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -1722,7 +1722,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -1730,7 +1730,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -1738,7 +1738,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -1746,7 +1746,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
@@ -1754,7 +1754,7 @@
         <v>102</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="117" customHeight="1" x14ac:dyDescent="0.3">
@@ -1762,7 +1762,7 @@
         <v>103</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1770,7 +1770,7 @@
         <v>104</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -1778,7 +1778,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -1786,7 +1786,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -1794,7 +1794,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -1802,7 +1802,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -1810,7 +1810,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -1818,7 +1818,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -1826,10 +1826,10 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C111" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -1837,7 +1837,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -1845,7 +1845,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -1853,7 +1853,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -1861,7 +1861,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
@@ -1869,7 +1869,7 @@
         <v>116</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="103.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -1877,7 +1877,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -1885,7 +1885,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>